<commit_message>
first functional version of the schema is done.
</commit_message>
<xml_diff>
--- a/issue-1249_prototyping_new_json_schema/field_descriptions.xlsx
+++ b/issue-1249_prototyping_new_json_schema/field_descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/project/random_notebooks/issue-1249_prototyping_new_json_schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BACEE4-A94C-BF4B-9672-670FF8E7AEE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2061D213-F59C-3945-A0BC-86EFCC97AC01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="960" windowWidth="28040" windowHeight="17040" xr2:uid="{B126AD1A-CC8D-1B4C-ACB9-8DD589ACB8CD}"/>
   </bookViews>
@@ -463,7 +463,7 @@
     <t>SO code of the functional consequence of the variant</t>
   </si>
   <si>
-    <t>"^rs[0-9]{1,}$"</t>
+    <t>^rs[0-9]{1,}$</t>
   </si>
 </sst>
 </file>
@@ -491,12 +491,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -511,10 +517,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,10 +840,10 @@
   <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A63" sqref="A63"/>
+      <selection pane="bottomRight" activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1021,31 +1029,37 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="J14" t="s">
+      <c r="H14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="J15" t="s">
+      <c r="H15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1061,39 +1075,48 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="4" t="str">
         <f>VLOOKUP(A17,Sheet2!A16:B91,2,FALSE)</f>
         <v>string</v>
       </c>
-      <c r="J17" t="s">
+      <c r="H17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B18" s="4" t="str">
         <f>VLOOKUP(A18,Sheet2!A17:B92,2,FALSE)</f>
         <v>string</v>
       </c>
-      <c r="J18" t="s">
+      <c r="H18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B19" s="4" t="str">
         <f>VLOOKUP(A19,Sheet2!A18:B93,2,FALSE)</f>
         <v>string</v>
       </c>
-      <c r="J19" t="s">
+      <c r="H19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1152,46 +1175,55 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="str">
+      <c r="B25" s="4" t="str">
         <f>VLOOKUP(A25,Sheet2!A24:B99,2,FALSE)</f>
         <v>string</v>
       </c>
-      <c r="J25" t="s">
+      <c r="H25" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="B26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="4">
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="4">
         <v>1</v>
       </c>
-      <c r="J27" t="s">
+      <c r="H27" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1217,17 +1249,20 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="J30" t="s">
+      <c r="H30" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1254,31 +1289,37 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="J33" t="s">
+      <c r="H33" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="J34" t="s">
+      <c r="H34" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1304,37 +1345,43 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="4">
         <v>0</v>
       </c>
-      <c r="J37" t="s">
+      <c r="H37" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="4">
         <v>0</v>
       </c>
-      <c r="J38" t="s">
+      <c r="H38" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1350,14 +1397,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="J40" t="s">
+      <c r="H40" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" s="4" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1385,18 +1435,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B43" t="str">
+      <c r="B43" s="4" t="str">
         <f>VLOOKUP(A43,Sheet2!A42:B117,2,FALSE)</f>
         <v>string</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="J43" t="s">
+      <c r="H43" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" s="4" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1412,31 +1465,37 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="4">
         <v>0</v>
       </c>
-      <c r="J45" t="s">
+      <c r="H45" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
-        <v>68</v>
-      </c>
-      <c r="J46" t="s">
+      <c r="B46" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H46" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" s="4" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1517,17 +1576,20 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="B54" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="J54" t="s">
+      <c r="H54" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1542,35 +1604,41 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B56" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="J56" t="s">
+      <c r="H56" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B57" t="str">
+      <c r="B57" s="4" t="str">
         <f>VLOOKUP(A57,Sheet2!A56:B131,2,FALSE)</f>
         <v>string</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="I57" t="s">
+      <c r="H57" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J57" s="4" t="s">
         <v>122</v>
       </c>
     </row>

</xml_diff>